<commit_message>
expand data type 01
</commit_message>
<xml_diff>
--- a/corpRch_ecoAct/data/분석_데이터_목록.xlsx
+++ b/corpRch_ecoAct/data/분석_데이터_목록.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="varInfo" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="79">
   <si>
     <t xml:space="preserve">순서</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t xml:space="preserve">Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">단위</t>
   </si>
   <si>
     <t xml:space="preserve">정상성</t>
@@ -78,6 +81,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구소</t>
     </r>
@@ -97,6 +101,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">수</t>
     </r>
@@ -114,6 +119,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">기업부설연구소</t>
     </r>
@@ -133,6 +139,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">정리</t>
     </r>
@@ -154,6 +161,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">한국산업진흥협회 월간 발표자료 </t>
     </r>
@@ -173,6 +181,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">자료실</t>
     </r>
@@ -194,6 +203,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">등록한 국내 기업 부설 연구소 월간 총계 및 분야별 집계</t>
     </r>
@@ -213,6 +223,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구원 집계</t>
     </r>
@@ -237,9 +248,13 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">개월</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">개소</t>
   </si>
   <si>
     <r>
@@ -248,6 +263,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구소</t>
     </r>
@@ -267,6 +283,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구원</t>
     </r>
@@ -286,9 +303,13 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">수</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">명</t>
   </si>
   <si>
     <r>
@@ -297,6 +318,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구소</t>
     </r>
@@ -316,6 +338,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">석박사</t>
     </r>
@@ -335,9 +358,13 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">비율</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
   </si>
   <si>
     <r>
@@ -346,6 +373,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구전담부서</t>
     </r>
@@ -365,6 +393,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">수</t>
     </r>
@@ -379,6 +408,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구전담부서</t>
     </r>
@@ -398,6 +428,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">정리</t>
     </r>
@@ -419,6 +450,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">등록한 국내 기업 연구전담부서 월간 총계 및 분야별 집계</t>
     </r>
@@ -438,6 +470,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구원 집계</t>
     </r>
@@ -449,6 +482,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구전담부서</t>
     </r>
@@ -468,6 +502,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구원</t>
     </r>
@@ -487,6 +522,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">수</t>
     </r>
@@ -498,6 +534,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구전담부서</t>
     </r>
@@ -517,6 +554,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">석박사</t>
     </r>
@@ -536,9 +574,94 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">비율</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">경제_사회_인구구조</t>
+  </si>
+  <si>
+    <t xml:space="preserve">경제활동인구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">경제 활동 역동성</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ecoAct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">취업자_경제활동인구_계절조정_수정.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">한국은행통계시스템</t>
+  </si>
+  <si>
+    <t xml:space="preserve">한국은행_거시경제지표_통계</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2개월</t>
+  </si>
+  <si>
+    <t xml:space="preserve">천명 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  취업자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">비임금근로자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">고용원이 있는 자영업자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">고용원이 없는 자영업자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">무급가족종사자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">임금근로자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">상용근로자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">임시근로자</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 일용근로자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">남자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">경제 활동 인구구조</t>
+  </si>
+  <si>
+    <t xml:space="preserve">여자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">실업자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">실업률</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15세이상인구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">비경제활동인구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">경제활동참가율</t>
+  </si>
+  <si>
+    <t xml:space="preserve">고용률</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
@@ -550,6 +673,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구소</t>
     </r>
@@ -569,6 +693,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">수</t>
     </r>
@@ -580,6 +705,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구소</t>
     </r>
@@ -599,6 +725,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구원</t>
     </r>
@@ -618,6 +745,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">수</t>
     </r>
@@ -629,6 +757,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구소</t>
     </r>
@@ -648,6 +777,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">석박사</t>
     </r>
@@ -667,6 +797,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">비율</t>
     </r>
@@ -678,6 +809,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구전담부서</t>
     </r>
@@ -697,6 +829,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">수</t>
     </r>
@@ -708,6 +841,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구전담부서</t>
     </r>
@@ -727,6 +861,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구원</t>
     </r>
@@ -746,6 +881,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">수</t>
     </r>
@@ -757,6 +893,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">연구전담부서</t>
     </r>
@@ -776,6 +913,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">석박사</t>
     </r>
@@ -795,6 +933,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK KR"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">비율</t>
     </r>
@@ -832,12 +971,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK KR"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -859,6 +999,13 @@
       <sz val="11"/>
       <name val="Noto Sans CJK KR"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Noto Sans CJK KR"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -874,6 +1021,18 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Noto Sans KR"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -883,7 +1042,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -896,6 +1055,19 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFDBDBDB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDBDBDB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFDBDBDB"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -924,24 +1096,68 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -954,6 +1170,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -962,328 +1238,1210 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.78125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1007" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="9.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="9.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="5" style="2" width="9.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="9.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1007" min="16" style="2" width="9.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1008" style="2" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="11" t="n">
+        <v>40544</v>
+      </c>
+      <c r="M2" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N2" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="11" t="n">
+        <v>40544</v>
+      </c>
+      <c r="M3" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N3" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="11" t="n">
+        <v>40544</v>
+      </c>
+      <c r="M4" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N4" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M5" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N5" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M6" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N6" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M7" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N7" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M8" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N8" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M9" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N9" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M10" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N10" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O10" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M11" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N11" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M12" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N12" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M13" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N13" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M14" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N14" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M15" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N15" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9" t="n">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M16" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N16" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O16" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9" t="n">
         <v>16</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M17" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N17" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O17" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="C18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L18" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M18" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N18" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O18" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="C19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M19" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N19" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="C20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L20" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M20" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N20" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O20" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="C21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M21" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N21" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O21" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="C22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M22" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N22" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O22" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" s="9" t="n">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="C23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="4" t="n">
-        <v>40544</v>
-      </c>
-      <c r="M2" s="4" t="n">
+      <c r="K23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L23" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M23" s="11" t="n">
         <v>46539</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N23" s="9" t="n">
         <v>162</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="O23" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" s="9" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L24" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M24" s="11" t="n">
+        <v>46539</v>
+      </c>
+      <c r="N24" s="9" t="n">
+        <v>162</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" s="9" t="n">
         <v>24</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="C25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="4" t="n">
-        <v>40544</v>
-      </c>
-      <c r="M3" s="4" t="n">
+      <c r="K25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L25" s="11" t="n">
+        <v>40545</v>
+      </c>
+      <c r="M25" s="11" t="n">
         <v>46539</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N25" s="9" t="n">
         <v>162</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="4" t="n">
-        <v>40544</v>
-      </c>
-      <c r="M4" s="4" t="n">
-        <v>46539</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="4" t="n">
-        <v>40545</v>
-      </c>
-      <c r="M5" s="4" t="n">
-        <v>46540</v>
-      </c>
-      <c r="N5" s="0" t="n">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="4" t="n">
-        <v>40545</v>
-      </c>
-      <c r="M6" s="4" t="n">
-        <v>46540</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="4" t="n">
-        <v>40545</v>
-      </c>
-      <c r="M7" s="4" t="n">
-        <v>46540</v>
-      </c>
-      <c r="N7" s="0" t="n">
-        <v>162</v>
-      </c>
-    </row>
+      <c r="O25" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1303,39 +2461,39 @@
   <dimension ref="A1:H163"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.7734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>38</v>
+      <c r="B1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="15" t="n">
         <v>40544</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -1358,10 +2516,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="15" t="n">
         <v>40575</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -1384,10 +2542,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="15" t="n">
         <v>40603</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -1410,10 +2568,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="15" t="n">
         <v>40634</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -1436,10 +2594,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="15" t="n">
         <v>40664</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -1462,10 +2620,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="15" t="n">
         <v>40695</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -1488,10 +2646,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="15" t="n">
         <v>40725</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -1514,10 +2672,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="15" t="n">
         <v>40756</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -1540,10 +2698,10 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="15" t="n">
         <v>40787</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -1566,10 +2724,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="15" t="n">
         <v>40817</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -1592,10 +2750,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="n">
+      <c r="B12" s="15" t="n">
         <v>40848</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -1618,10 +2776,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="n">
+      <c r="B13" s="15" t="n">
         <v>40878</v>
       </c>
       <c r="C13" s="0" t="n">
@@ -1644,10 +2802,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="n">
+      <c r="B14" s="15" t="n">
         <v>40909</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -1670,10 +2828,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="n">
+      <c r="B15" s="15" t="n">
         <v>40940</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -1696,10 +2854,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="n">
+      <c r="B16" s="15" t="n">
         <v>40969</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -1722,10 +2880,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="n">
+      <c r="B17" s="15" t="n">
         <v>41000</v>
       </c>
       <c r="C17" s="0" t="n">
@@ -1748,10 +2906,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="n">
+      <c r="B18" s="15" t="n">
         <v>41030</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -1774,10 +2932,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="n">
+      <c r="B19" s="15" t="n">
         <v>41061</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -1800,10 +2958,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="n">
+      <c r="B20" s="15" t="n">
         <v>41091</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -1826,10 +2984,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="n">
+      <c r="B21" s="15" t="n">
         <v>41122</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -1852,10 +3010,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="4" t="n">
+      <c r="B22" s="15" t="n">
         <v>41153</v>
       </c>
       <c r="C22" s="0" t="n">
@@ -1878,10 +3036,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="4" t="n">
+      <c r="B23" s="15" t="n">
         <v>41183</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -1904,10 +3062,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="4" t="n">
+      <c r="B24" s="15" t="n">
         <v>41214</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -1930,10 +3088,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="4" t="n">
+      <c r="B25" s="15" t="n">
         <v>41244</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -1956,10 +3114,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="5" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="4" t="n">
+      <c r="B26" s="15" t="n">
         <v>41275</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -1982,10 +3140,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="4" t="n">
+      <c r="B27" s="15" t="n">
         <v>41306</v>
       </c>
       <c r="C27" s="0" t="n">
@@ -2008,10 +3166,10 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="4" t="n">
+      <c r="B28" s="15" t="n">
         <v>41334</v>
       </c>
       <c r="C28" s="0" t="n">
@@ -2034,10 +3192,10 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="B29" s="4" t="n">
+      <c r="B29" s="15" t="n">
         <v>41365</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -2060,10 +3218,10 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="5" t="n">
         <v>28</v>
       </c>
-      <c r="B30" s="4" t="n">
+      <c r="B30" s="15" t="n">
         <v>41395</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -2086,10 +3244,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="5" t="n">
         <v>29</v>
       </c>
-      <c r="B31" s="4" t="n">
+      <c r="B31" s="15" t="n">
         <v>41426</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -2112,10 +3270,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="B32" s="4" t="n">
+      <c r="B32" s="15" t="n">
         <v>41456</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -2138,10 +3296,10 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="B33" s="4" t="n">
+      <c r="B33" s="15" t="n">
         <v>41487</v>
       </c>
       <c r="C33" s="0" t="n">
@@ -2164,10 +3322,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="B34" s="4" t="n">
+      <c r="B34" s="15" t="n">
         <v>41518</v>
       </c>
       <c r="C34" s="0" t="n">
@@ -2190,10 +3348,10 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="4" t="n">
+      <c r="B35" s="15" t="n">
         <v>41548</v>
       </c>
       <c r="C35" s="0" t="n">
@@ -2216,10 +3374,10 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="4" t="n">
+      <c r="B36" s="15" t="n">
         <v>41579</v>
       </c>
       <c r="C36" s="0" t="n">
@@ -2242,10 +3400,10 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="4" t="n">
+      <c r="B37" s="15" t="n">
         <v>41609</v>
       </c>
       <c r="C37" s="0" t="n">
@@ -2268,10 +3426,10 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="B38" s="4" t="n">
+      <c r="B38" s="15" t="n">
         <v>41640</v>
       </c>
       <c r="C38" s="0" t="n">
@@ -2294,10 +3452,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="4" t="n">
+      <c r="B39" s="15" t="n">
         <v>41671</v>
       </c>
       <c r="C39" s="0" t="n">
@@ -2320,10 +3478,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="4" t="n">
+      <c r="B40" s="15" t="n">
         <v>41699</v>
       </c>
       <c r="C40" s="0" t="n">
@@ -2346,10 +3504,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="4" t="n">
+      <c r="B41" s="15" t="n">
         <v>41730</v>
       </c>
       <c r="C41" s="0" t="n">
@@ -2372,10 +3530,10 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="B42" s="4" t="n">
+      <c r="B42" s="15" t="n">
         <v>41760</v>
       </c>
       <c r="C42" s="0" t="n">
@@ -2398,10 +3556,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="B43" s="4" t="n">
+      <c r="B43" s="15" t="n">
         <v>41791</v>
       </c>
       <c r="C43" s="0" t="n">
@@ -2424,10 +3582,10 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="5" t="n">
         <v>42</v>
       </c>
-      <c r="B44" s="4" t="n">
+      <c r="B44" s="15" t="n">
         <v>41821</v>
       </c>
       <c r="C44" s="0" t="n">
@@ -2450,10 +3608,10 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="5" t="n">
         <v>43</v>
       </c>
-      <c r="B45" s="4" t="n">
+      <c r="B45" s="15" t="n">
         <v>41852</v>
       </c>
       <c r="C45" s="0" t="n">
@@ -2476,10 +3634,10 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="B46" s="4" t="n">
+      <c r="B46" s="15" t="n">
         <v>41883</v>
       </c>
       <c r="C46" s="0" t="n">
@@ -2502,10 +3660,10 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="B47" s="4" t="n">
+      <c r="B47" s="15" t="n">
         <v>41913</v>
       </c>
       <c r="C47" s="0" t="n">
@@ -2528,10 +3686,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="5" t="n">
         <v>46</v>
       </c>
-      <c r="B48" s="4" t="n">
+      <c r="B48" s="15" t="n">
         <v>41944</v>
       </c>
       <c r="C48" s="0" t="n">
@@ -2554,10 +3712,10 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+      <c r="A49" s="5" t="n">
         <v>47</v>
       </c>
-      <c r="B49" s="4" t="n">
+      <c r="B49" s="15" t="n">
         <v>41974</v>
       </c>
       <c r="C49" s="0" t="n">
@@ -2580,10 +3738,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
+      <c r="A50" s="5" t="n">
         <v>48</v>
       </c>
-      <c r="B50" s="4" t="n">
+      <c r="B50" s="15" t="n">
         <v>42005</v>
       </c>
       <c r="C50" s="0" t="n">
@@ -2606,10 +3764,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
+      <c r="A51" s="5" t="n">
         <v>49</v>
       </c>
-      <c r="B51" s="4" t="n">
+      <c r="B51" s="15" t="n">
         <v>42036</v>
       </c>
       <c r="C51" s="0" t="n">
@@ -2632,10 +3790,10 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
+      <c r="A52" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="B52" s="4" t="n">
+      <c r="B52" s="15" t="n">
         <v>42064</v>
       </c>
       <c r="C52" s="0" t="n">
@@ -2658,10 +3816,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
+      <c r="A53" s="5" t="n">
         <v>51</v>
       </c>
-      <c r="B53" s="4" t="n">
+      <c r="B53" s="15" t="n">
         <v>42095</v>
       </c>
       <c r="C53" s="0" t="n">
@@ -2684,10 +3842,10 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="5" t="n">
         <v>52</v>
       </c>
-      <c r="B54" s="4" t="n">
+      <c r="B54" s="15" t="n">
         <v>42125</v>
       </c>
       <c r="C54" s="0" t="n">
@@ -2710,10 +3868,10 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="5" t="n">
         <v>53</v>
       </c>
-      <c r="B55" s="4" t="n">
+      <c r="B55" s="15" t="n">
         <v>42156</v>
       </c>
       <c r="C55" s="0" t="n">
@@ -2736,10 +3894,10 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="5" t="n">
         <v>54</v>
       </c>
-      <c r="B56" s="4" t="n">
+      <c r="B56" s="15" t="n">
         <v>42186</v>
       </c>
       <c r="C56" s="0" t="n">
@@ -2762,10 +3920,10 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="5" t="n">
         <v>55</v>
       </c>
-      <c r="B57" s="4" t="n">
+      <c r="B57" s="15" t="n">
         <v>42217</v>
       </c>
       <c r="C57" s="0" t="n">
@@ -2788,10 +3946,10 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="5" t="n">
         <v>56</v>
       </c>
-      <c r="B58" s="4" t="n">
+      <c r="B58" s="15" t="n">
         <v>42248</v>
       </c>
       <c r="C58" s="0" t="n">
@@ -2814,10 +3972,10 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="5" t="n">
         <v>57</v>
       </c>
-      <c r="B59" s="4" t="n">
+      <c r="B59" s="15" t="n">
         <v>42278</v>
       </c>
       <c r="C59" s="0" t="n">
@@ -2840,10 +3998,10 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="5" t="n">
         <v>58</v>
       </c>
-      <c r="B60" s="4" t="n">
+      <c r="B60" s="15" t="n">
         <v>42309</v>
       </c>
       <c r="C60" s="0" t="n">
@@ -2866,10 +4024,10 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="5" t="n">
         <v>59</v>
       </c>
-      <c r="B61" s="4" t="n">
+      <c r="B61" s="15" t="n">
         <v>42339</v>
       </c>
       <c r="C61" s="0" t="n">
@@ -2892,10 +4050,10 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="B62" s="4" t="n">
+      <c r="B62" s="15" t="n">
         <v>42370</v>
       </c>
       <c r="C62" s="0" t="n">
@@ -2918,10 +4076,10 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="5" t="n">
         <v>61</v>
       </c>
-      <c r="B63" s="4" t="n">
+      <c r="B63" s="15" t="n">
         <v>42401</v>
       </c>
       <c r="C63" s="0" t="n">
@@ -2944,10 +4102,10 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="5" t="n">
         <v>62</v>
       </c>
-      <c r="B64" s="4" t="n">
+      <c r="B64" s="15" t="n">
         <v>42430</v>
       </c>
       <c r="C64" s="0" t="n">
@@ -2970,10 +4128,10 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="5" t="n">
         <v>63</v>
       </c>
-      <c r="B65" s="4" t="n">
+      <c r="B65" s="15" t="n">
         <v>42461</v>
       </c>
       <c r="C65" s="0" t="n">
@@ -2996,10 +4154,10 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="5" t="n">
         <v>64</v>
       </c>
-      <c r="B66" s="4" t="n">
+      <c r="B66" s="15" t="n">
         <v>42491</v>
       </c>
       <c r="C66" s="0" t="n">
@@ -3022,10 +4180,10 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
+      <c r="A67" s="5" t="n">
         <v>65</v>
       </c>
-      <c r="B67" s="4" t="n">
+      <c r="B67" s="15" t="n">
         <v>42522</v>
       </c>
       <c r="C67" s="0" t="n">
@@ -3048,10 +4206,10 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
+      <c r="A68" s="5" t="n">
         <v>66</v>
       </c>
-      <c r="B68" s="4" t="n">
+      <c r="B68" s="15" t="n">
         <v>42552</v>
       </c>
       <c r="C68" s="0" t="n">
@@ -3074,10 +4232,10 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
+      <c r="A69" s="5" t="n">
         <v>67</v>
       </c>
-      <c r="B69" s="4" t="n">
+      <c r="B69" s="15" t="n">
         <v>42583</v>
       </c>
       <c r="C69" s="0" t="n">
@@ -3100,10 +4258,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
+      <c r="A70" s="5" t="n">
         <v>68</v>
       </c>
-      <c r="B70" s="4" t="n">
+      <c r="B70" s="15" t="n">
         <v>42614</v>
       </c>
       <c r="C70" s="0" t="n">
@@ -3126,10 +4284,10 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
+      <c r="A71" s="5" t="n">
         <v>69</v>
       </c>
-      <c r="B71" s="4" t="n">
+      <c r="B71" s="15" t="n">
         <v>42644</v>
       </c>
       <c r="C71" s="0" t="n">
@@ -3152,10 +4310,10 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
+      <c r="A72" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="B72" s="4" t="n">
+      <c r="B72" s="15" t="n">
         <v>42675</v>
       </c>
       <c r="C72" s="0" t="n">
@@ -3178,10 +4336,10 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="n">
+      <c r="A73" s="5" t="n">
         <v>71</v>
       </c>
-      <c r="B73" s="4" t="n">
+      <c r="B73" s="15" t="n">
         <v>42705</v>
       </c>
       <c r="C73" s="0" t="n">
@@ -3204,10 +4362,10 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
+      <c r="A74" s="5" t="n">
         <v>72</v>
       </c>
-      <c r="B74" s="4" t="n">
+      <c r="B74" s="15" t="n">
         <v>42736</v>
       </c>
       <c r="C74" s="0" t="n">
@@ -3230,10 +4388,10 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
+      <c r="A75" s="5" t="n">
         <v>73</v>
       </c>
-      <c r="B75" s="4" t="n">
+      <c r="B75" s="15" t="n">
         <v>42767</v>
       </c>
       <c r="C75" s="0" t="n">
@@ -3256,10 +4414,10 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="n">
+      <c r="A76" s="5" t="n">
         <v>74</v>
       </c>
-      <c r="B76" s="4" t="n">
+      <c r="B76" s="15" t="n">
         <v>42795</v>
       </c>
       <c r="C76" s="0" t="n">
@@ -3282,10 +4440,10 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="n">
+      <c r="A77" s="5" t="n">
         <v>75</v>
       </c>
-      <c r="B77" s="4" t="n">
+      <c r="B77" s="15" t="n">
         <v>42826</v>
       </c>
       <c r="C77" s="0" t="n">
@@ -3308,10 +4466,10 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="n">
+      <c r="A78" s="5" t="n">
         <v>76</v>
       </c>
-      <c r="B78" s="4" t="n">
+      <c r="B78" s="15" t="n">
         <v>42856</v>
       </c>
       <c r="C78" s="0" t="n">
@@ -3334,10 +4492,10 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
+      <c r="A79" s="5" t="n">
         <v>77</v>
       </c>
-      <c r="B79" s="4" t="n">
+      <c r="B79" s="15" t="n">
         <v>42887</v>
       </c>
       <c r="C79" s="0" t="n">
@@ -3360,10 +4518,10 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
+      <c r="A80" s="5" t="n">
         <v>78</v>
       </c>
-      <c r="B80" s="4" t="n">
+      <c r="B80" s="15" t="n">
         <v>42917</v>
       </c>
       <c r="C80" s="0" t="n">
@@ -3386,10 +4544,10 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="n">
+      <c r="A81" s="5" t="n">
         <v>79</v>
       </c>
-      <c r="B81" s="4" t="n">
+      <c r="B81" s="15" t="n">
         <v>42948</v>
       </c>
       <c r="C81" s="0" t="n">
@@ -3412,10 +4570,10 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="n">
+      <c r="A82" s="5" t="n">
         <v>80</v>
       </c>
-      <c r="B82" s="4" t="n">
+      <c r="B82" s="15" t="n">
         <v>42979</v>
       </c>
       <c r="C82" s="0" t="n">
@@ -3438,10 +4596,10 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
+      <c r="A83" s="5" t="n">
         <v>81</v>
       </c>
-      <c r="B83" s="4" t="n">
+      <c r="B83" s="15" t="n">
         <v>43009</v>
       </c>
       <c r="C83" s="0" t="n">
@@ -3464,10 +4622,10 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
+      <c r="A84" s="5" t="n">
         <v>82</v>
       </c>
-      <c r="B84" s="4" t="n">
+      <c r="B84" s="15" t="n">
         <v>43040</v>
       </c>
       <c r="C84" s="0" t="n">
@@ -3490,10 +4648,10 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
+      <c r="A85" s="5" t="n">
         <v>83</v>
       </c>
-      <c r="B85" s="4" t="n">
+      <c r="B85" s="15" t="n">
         <v>43070</v>
       </c>
       <c r="C85" s="0" t="n">
@@ -3516,10 +4674,10 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
+      <c r="A86" s="5" t="n">
         <v>84</v>
       </c>
-      <c r="B86" s="4" t="n">
+      <c r="B86" s="15" t="n">
         <v>43101</v>
       </c>
       <c r="C86" s="0" t="n">
@@ -3542,10 +4700,10 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
+      <c r="A87" s="5" t="n">
         <v>85</v>
       </c>
-      <c r="B87" s="4" t="n">
+      <c r="B87" s="15" t="n">
         <v>43132</v>
       </c>
       <c r="C87" s="0" t="n">
@@ -3568,10 +4726,10 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
+      <c r="A88" s="5" t="n">
         <v>86</v>
       </c>
-      <c r="B88" s="4" t="n">
+      <c r="B88" s="15" t="n">
         <v>43160</v>
       </c>
       <c r="C88" s="0" t="n">
@@ -3594,10 +4752,10 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
+      <c r="A89" s="5" t="n">
         <v>87</v>
       </c>
-      <c r="B89" s="4" t="n">
+      <c r="B89" s="15" t="n">
         <v>43191</v>
       </c>
       <c r="C89" s="0" t="n">
@@ -3620,10 +4778,10 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
+      <c r="A90" s="5" t="n">
         <v>88</v>
       </c>
-      <c r="B90" s="4" t="n">
+      <c r="B90" s="15" t="n">
         <v>43221</v>
       </c>
       <c r="C90" s="0" t="n">
@@ -3646,10 +4804,10 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="n">
+      <c r="A91" s="5" t="n">
         <v>89</v>
       </c>
-      <c r="B91" s="4" t="n">
+      <c r="B91" s="15" t="n">
         <v>43252</v>
       </c>
       <c r="C91" s="0" t="n">
@@ -3672,10 +4830,10 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="n">
+      <c r="A92" s="5" t="n">
         <v>90</v>
       </c>
-      <c r="B92" s="4" t="n">
+      <c r="B92" s="15" t="n">
         <v>43282</v>
       </c>
       <c r="C92" s="0" t="n">
@@ -3698,10 +4856,10 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="n">
+      <c r="A93" s="5" t="n">
         <v>91</v>
       </c>
-      <c r="B93" s="4" t="n">
+      <c r="B93" s="15" t="n">
         <v>43313</v>
       </c>
       <c r="C93" s="0" t="n">
@@ -3724,10 +4882,10 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="n">
+      <c r="A94" s="5" t="n">
         <v>92</v>
       </c>
-      <c r="B94" s="4" t="n">
+      <c r="B94" s="15" t="n">
         <v>43344</v>
       </c>
       <c r="C94" s="0" t="n">
@@ -3750,10 +4908,10 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="n">
+      <c r="A95" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="B95" s="4" t="n">
+      <c r="B95" s="15" t="n">
         <v>43374</v>
       </c>
       <c r="C95" s="0" t="n">
@@ -3776,10 +4934,10 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="n">
+      <c r="A96" s="5" t="n">
         <v>94</v>
       </c>
-      <c r="B96" s="4" t="n">
+      <c r="B96" s="15" t="n">
         <v>43405</v>
       </c>
       <c r="C96" s="0" t="n">
@@ -3802,10 +4960,10 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="n">
+      <c r="A97" s="5" t="n">
         <v>95</v>
       </c>
-      <c r="B97" s="4" t="n">
+      <c r="B97" s="15" t="n">
         <v>43435</v>
       </c>
       <c r="C97" s="0" t="n">
@@ -3828,10 +4986,10 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="n">
+      <c r="A98" s="5" t="n">
         <v>96</v>
       </c>
-      <c r="B98" s="4" t="n">
+      <c r="B98" s="15" t="n">
         <v>43466</v>
       </c>
       <c r="C98" s="0" t="n">
@@ -3854,10 +5012,10 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="n">
+      <c r="A99" s="5" t="n">
         <v>97</v>
       </c>
-      <c r="B99" s="4" t="n">
+      <c r="B99" s="15" t="n">
         <v>43497</v>
       </c>
       <c r="C99" s="0" t="n">
@@ -3880,10 +5038,10 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="n">
+      <c r="A100" s="5" t="n">
         <v>98</v>
       </c>
-      <c r="B100" s="4" t="n">
+      <c r="B100" s="15" t="n">
         <v>43525</v>
       </c>
       <c r="C100" s="0" t="n">
@@ -3906,10 +5064,10 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
+      <c r="A101" s="5" t="n">
         <v>99</v>
       </c>
-      <c r="B101" s="4" t="n">
+      <c r="B101" s="15" t="n">
         <v>43556</v>
       </c>
       <c r="C101" s="0" t="n">
@@ -3932,10 +5090,10 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1" t="n">
+      <c r="A102" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="B102" s="4" t="n">
+      <c r="B102" s="15" t="n">
         <v>43586</v>
       </c>
       <c r="C102" s="0" t="n">
@@ -3958,10 +5116,10 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="n">
+      <c r="A103" s="5" t="n">
         <v>101</v>
       </c>
-      <c r="B103" s="4" t="n">
+      <c r="B103" s="15" t="n">
         <v>43617</v>
       </c>
       <c r="C103" s="0" t="n">
@@ -3984,10 +5142,10 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="n">
+      <c r="A104" s="5" t="n">
         <v>102</v>
       </c>
-      <c r="B104" s="4" t="n">
+      <c r="B104" s="15" t="n">
         <v>43647</v>
       </c>
       <c r="C104" s="0" t="n">
@@ -4010,10 +5168,10 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="n">
+      <c r="A105" s="5" t="n">
         <v>103</v>
       </c>
-      <c r="B105" s="4" t="n">
+      <c r="B105" s="15" t="n">
         <v>43678</v>
       </c>
       <c r="C105" s="0" t="n">
@@ -4036,10 +5194,10 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="n">
+      <c r="A106" s="5" t="n">
         <v>104</v>
       </c>
-      <c r="B106" s="4" t="n">
+      <c r="B106" s="15" t="n">
         <v>43709</v>
       </c>
       <c r="C106" s="0" t="n">
@@ -4062,10 +5220,10 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="n">
+      <c r="A107" s="5" t="n">
         <v>105</v>
       </c>
-      <c r="B107" s="4" t="n">
+      <c r="B107" s="15" t="n">
         <v>43739</v>
       </c>
       <c r="C107" s="0" t="n">
@@ -4088,10 +5246,10 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="n">
+      <c r="A108" s="5" t="n">
         <v>106</v>
       </c>
-      <c r="B108" s="4" t="n">
+      <c r="B108" s="15" t="n">
         <v>43770</v>
       </c>
       <c r="C108" s="0" t="n">
@@ -4114,10 +5272,10 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="n">
+      <c r="A109" s="5" t="n">
         <v>107</v>
       </c>
-      <c r="B109" s="4" t="n">
+      <c r="B109" s="15" t="n">
         <v>43800</v>
       </c>
       <c r="C109" s="0" t="n">
@@ -4140,10 +5298,10 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="n">
+      <c r="A110" s="5" t="n">
         <v>108</v>
       </c>
-      <c r="B110" s="4" t="n">
+      <c r="B110" s="15" t="n">
         <v>43831</v>
       </c>
       <c r="C110" s="0" t="n">
@@ -4166,10 +5324,10 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="n">
+      <c r="A111" s="5" t="n">
         <v>109</v>
       </c>
-      <c r="B111" s="4" t="n">
+      <c r="B111" s="15" t="n">
         <v>43862</v>
       </c>
       <c r="C111" s="0" t="n">
@@ -4192,10 +5350,10 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="n">
+      <c r="A112" s="5" t="n">
         <v>110</v>
       </c>
-      <c r="B112" s="4" t="n">
+      <c r="B112" s="15" t="n">
         <v>43891</v>
       </c>
       <c r="C112" s="0" t="n">
@@ -4218,10 +5376,10 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="n">
+      <c r="A113" s="5" t="n">
         <v>111</v>
       </c>
-      <c r="B113" s="4" t="n">
+      <c r="B113" s="15" t="n">
         <v>43922</v>
       </c>
       <c r="C113" s="0" t="n">
@@ -4244,10 +5402,10 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="n">
+      <c r="A114" s="5" t="n">
         <v>112</v>
       </c>
-      <c r="B114" s="4" t="n">
+      <c r="B114" s="15" t="n">
         <v>43952</v>
       </c>
       <c r="C114" s="0" t="n">
@@ -4270,10 +5428,10 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="n">
+      <c r="A115" s="5" t="n">
         <v>113</v>
       </c>
-      <c r="B115" s="4" t="n">
+      <c r="B115" s="15" t="n">
         <v>43983</v>
       </c>
       <c r="C115" s="0" t="n">
@@ -4296,10 +5454,10 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="1" t="n">
+      <c r="A116" s="5" t="n">
         <v>114</v>
       </c>
-      <c r="B116" s="4" t="n">
+      <c r="B116" s="15" t="n">
         <v>44013</v>
       </c>
       <c r="C116" s="0" t="n">
@@ -4322,10 +5480,10 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="n">
+      <c r="A117" s="5" t="n">
         <v>115</v>
       </c>
-      <c r="B117" s="4" t="n">
+      <c r="B117" s="15" t="n">
         <v>44044</v>
       </c>
       <c r="C117" s="0" t="n">
@@ -4348,10 +5506,10 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="n">
+      <c r="A118" s="5" t="n">
         <v>116</v>
       </c>
-      <c r="B118" s="4" t="n">
+      <c r="B118" s="15" t="n">
         <v>44075</v>
       </c>
       <c r="C118" s="0" t="n">
@@ -4374,10 +5532,10 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="n">
+      <c r="A119" s="5" t="n">
         <v>117</v>
       </c>
-      <c r="B119" s="4" t="n">
+      <c r="B119" s="15" t="n">
         <v>44105</v>
       </c>
       <c r="C119" s="0" t="n">
@@ -4400,10 +5558,10 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="n">
+      <c r="A120" s="5" t="n">
         <v>118</v>
       </c>
-      <c r="B120" s="4" t="n">
+      <c r="B120" s="15" t="n">
         <v>44136</v>
       </c>
       <c r="C120" s="0" t="n">
@@ -4426,10 +5584,10 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="n">
+      <c r="A121" s="5" t="n">
         <v>119</v>
       </c>
-      <c r="B121" s="4" t="n">
+      <c r="B121" s="15" t="n">
         <v>44166</v>
       </c>
       <c r="C121" s="0" t="n">
@@ -4452,10 +5610,10 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="n">
+      <c r="A122" s="5" t="n">
         <v>120</v>
       </c>
-      <c r="B122" s="4" t="n">
+      <c r="B122" s="15" t="n">
         <v>44197</v>
       </c>
       <c r="C122" s="0" t="n">
@@ -4478,10 +5636,10 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="n">
+      <c r="A123" s="5" t="n">
         <v>121</v>
       </c>
-      <c r="B123" s="4" t="n">
+      <c r="B123" s="15" t="n">
         <v>44228</v>
       </c>
       <c r="C123" s="0" t="n">
@@ -4504,10 +5662,10 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="n">
+      <c r="A124" s="5" t="n">
         <v>122</v>
       </c>
-      <c r="B124" s="4" t="n">
+      <c r="B124" s="15" t="n">
         <v>44256</v>
       </c>
       <c r="C124" s="0" t="n">
@@ -4530,10 +5688,10 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="n">
+      <c r="A125" s="5" t="n">
         <v>123</v>
       </c>
-      <c r="B125" s="4" t="n">
+      <c r="B125" s="15" t="n">
         <v>44287</v>
       </c>
       <c r="C125" s="0" t="n">
@@ -4556,10 +5714,10 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="n">
+      <c r="A126" s="5" t="n">
         <v>124</v>
       </c>
-      <c r="B126" s="4" t="n">
+      <c r="B126" s="15" t="n">
         <v>44317</v>
       </c>
       <c r="C126" s="0" t="n">
@@ -4582,10 +5740,10 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="n">
+      <c r="A127" s="5" t="n">
         <v>125</v>
       </c>
-      <c r="B127" s="4" t="n">
+      <c r="B127" s="15" t="n">
         <v>44348</v>
       </c>
       <c r="C127" s="0" t="n">
@@ -4608,10 +5766,10 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="n">
+      <c r="A128" s="5" t="n">
         <v>126</v>
       </c>
-      <c r="B128" s="4" t="n">
+      <c r="B128" s="15" t="n">
         <v>44378</v>
       </c>
       <c r="C128" s="0" t="n">
@@ -4634,10 +5792,10 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="n">
+      <c r="A129" s="5" t="n">
         <v>127</v>
       </c>
-      <c r="B129" s="4" t="n">
+      <c r="B129" s="15" t="n">
         <v>44409</v>
       </c>
       <c r="C129" s="0" t="n">
@@ -4660,10 +5818,10 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="n">
+      <c r="A130" s="5" t="n">
         <v>128</v>
       </c>
-      <c r="B130" s="4" t="n">
+      <c r="B130" s="15" t="n">
         <v>44440</v>
       </c>
       <c r="C130" s="0" t="n">
@@ -4686,10 +5844,10 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="n">
+      <c r="A131" s="5" t="n">
         <v>129</v>
       </c>
-      <c r="B131" s="4" t="n">
+      <c r="B131" s="15" t="n">
         <v>44470</v>
       </c>
       <c r="C131" s="0" t="n">
@@ -4712,10 +5870,10 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="n">
+      <c r="A132" s="5" t="n">
         <v>130</v>
       </c>
-      <c r="B132" s="4" t="n">
+      <c r="B132" s="15" t="n">
         <v>44501</v>
       </c>
       <c r="C132" s="0" t="n">
@@ -4738,10 +5896,10 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="n">
+      <c r="A133" s="5" t="n">
         <v>131</v>
       </c>
-      <c r="B133" s="4" t="n">
+      <c r="B133" s="15" t="n">
         <v>44531</v>
       </c>
       <c r="C133" s="0" t="n">
@@ -4764,10 +5922,10 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="n">
+      <c r="A134" s="5" t="n">
         <v>132</v>
       </c>
-      <c r="B134" s="4" t="n">
+      <c r="B134" s="15" t="n">
         <v>44562</v>
       </c>
       <c r="C134" s="0" t="n">
@@ -4790,10 +5948,10 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="n">
+      <c r="A135" s="5" t="n">
         <v>133</v>
       </c>
-      <c r="B135" s="4" t="n">
+      <c r="B135" s="15" t="n">
         <v>44593</v>
       </c>
       <c r="C135" s="0" t="n">
@@ -4816,10 +5974,10 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="n">
+      <c r="A136" s="5" t="n">
         <v>134</v>
       </c>
-      <c r="B136" s="4" t="n">
+      <c r="B136" s="15" t="n">
         <v>44621</v>
       </c>
       <c r="C136" s="0" t="n">
@@ -4842,10 +6000,10 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="n">
+      <c r="A137" s="5" t="n">
         <v>135</v>
       </c>
-      <c r="B137" s="4" t="n">
+      <c r="B137" s="15" t="n">
         <v>44652</v>
       </c>
       <c r="C137" s="0" t="n">
@@ -4868,10 +6026,10 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="n">
+      <c r="A138" s="5" t="n">
         <v>136</v>
       </c>
-      <c r="B138" s="4" t="n">
+      <c r="B138" s="15" t="n">
         <v>44682</v>
       </c>
       <c r="C138" s="0" t="n">
@@ -4894,10 +6052,10 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="n">
+      <c r="A139" s="5" t="n">
         <v>137</v>
       </c>
-      <c r="B139" s="4" t="n">
+      <c r="B139" s="15" t="n">
         <v>44713</v>
       </c>
       <c r="C139" s="0" t="n">
@@ -4920,10 +6078,10 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="n">
+      <c r="A140" s="5" t="n">
         <v>138</v>
       </c>
-      <c r="B140" s="4" t="n">
+      <c r="B140" s="15" t="n">
         <v>44743</v>
       </c>
       <c r="C140" s="0" t="n">
@@ -4946,10 +6104,10 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="n">
+      <c r="A141" s="5" t="n">
         <v>139</v>
       </c>
-      <c r="B141" s="4" t="n">
+      <c r="B141" s="15" t="n">
         <v>44774</v>
       </c>
       <c r="C141" s="0" t="n">
@@ -4972,10 +6130,10 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="n">
+      <c r="A142" s="5" t="n">
         <v>140</v>
       </c>
-      <c r="B142" s="4" t="n">
+      <c r="B142" s="15" t="n">
         <v>44805</v>
       </c>
       <c r="C142" s="0" t="n">
@@ -4998,10 +6156,10 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="n">
+      <c r="A143" s="5" t="n">
         <v>141</v>
       </c>
-      <c r="B143" s="4" t="n">
+      <c r="B143" s="15" t="n">
         <v>44835</v>
       </c>
       <c r="C143" s="0" t="n">
@@ -5024,10 +6182,10 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="n">
+      <c r="A144" s="5" t="n">
         <v>142</v>
       </c>
-      <c r="B144" s="4" t="n">
+      <c r="B144" s="15" t="n">
         <v>44866</v>
       </c>
       <c r="C144" s="0" t="n">
@@ -5050,10 +6208,10 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="n">
+      <c r="A145" s="5" t="n">
         <v>143</v>
       </c>
-      <c r="B145" s="4" t="n">
+      <c r="B145" s="15" t="n">
         <v>44896</v>
       </c>
       <c r="C145" s="0" t="n">
@@ -5076,10 +6234,10 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="n">
+      <c r="A146" s="5" t="n">
         <v>144</v>
       </c>
-      <c r="B146" s="4" t="n">
+      <c r="B146" s="15" t="n">
         <v>44927</v>
       </c>
       <c r="C146" s="0" t="n">
@@ -5102,10 +6260,10 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="n">
+      <c r="A147" s="5" t="n">
         <v>145</v>
       </c>
-      <c r="B147" s="4" t="n">
+      <c r="B147" s="15" t="n">
         <v>44958</v>
       </c>
       <c r="C147" s="0" t="n">
@@ -5128,10 +6286,10 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="n">
+      <c r="A148" s="5" t="n">
         <v>146</v>
       </c>
-      <c r="B148" s="4" t="n">
+      <c r="B148" s="15" t="n">
         <v>44986</v>
       </c>
       <c r="C148" s="0" t="n">
@@ -5154,10 +6312,10 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="1" t="n">
+      <c r="A149" s="5" t="n">
         <v>147</v>
       </c>
-      <c r="B149" s="4" t="n">
+      <c r="B149" s="15" t="n">
         <v>45017</v>
       </c>
       <c r="C149" s="0" t="n">
@@ -5180,10 +6338,10 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="n">
+      <c r="A150" s="5" t="n">
         <v>148</v>
       </c>
-      <c r="B150" s="4" t="n">
+      <c r="B150" s="15" t="n">
         <v>45047</v>
       </c>
       <c r="C150" s="0" t="n">
@@ -5206,10 +6364,10 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="n">
+      <c r="A151" s="5" t="n">
         <v>149</v>
       </c>
-      <c r="B151" s="4" t="n">
+      <c r="B151" s="15" t="n">
         <v>45078</v>
       </c>
       <c r="C151" s="0" t="n">
@@ -5232,10 +6390,10 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="n">
+      <c r="A152" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="B152" s="4" t="n">
+      <c r="B152" s="15" t="n">
         <v>45108</v>
       </c>
       <c r="C152" s="0" t="n">
@@ -5258,10 +6416,10 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="n">
+      <c r="A153" s="5" t="n">
         <v>151</v>
       </c>
-      <c r="B153" s="4" t="n">
+      <c r="B153" s="15" t="n">
         <v>45139</v>
       </c>
       <c r="C153" s="0" t="n">
@@ -5284,10 +6442,10 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="n">
+      <c r="A154" s="5" t="n">
         <v>152</v>
       </c>
-      <c r="B154" s="4" t="n">
+      <c r="B154" s="15" t="n">
         <v>45170</v>
       </c>
       <c r="C154" s="0" t="n">
@@ -5310,10 +6468,10 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="n">
+      <c r="A155" s="5" t="n">
         <v>153</v>
       </c>
-      <c r="B155" s="4" t="n">
+      <c r="B155" s="15" t="n">
         <v>45200</v>
       </c>
       <c r="C155" s="0" t="n">
@@ -5336,10 +6494,10 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="n">
+      <c r="A156" s="5" t="n">
         <v>154</v>
       </c>
-      <c r="B156" s="4" t="n">
+      <c r="B156" s="15" t="n">
         <v>45231</v>
       </c>
       <c r="C156" s="0" t="n">
@@ -5362,10 +6520,10 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="n">
+      <c r="A157" s="5" t="n">
         <v>155</v>
       </c>
-      <c r="B157" s="4" t="n">
+      <c r="B157" s="15" t="n">
         <v>45261</v>
       </c>
       <c r="C157" s="0" t="n">
@@ -5388,10 +6546,10 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="n">
+      <c r="A158" s="5" t="n">
         <v>156</v>
       </c>
-      <c r="B158" s="4" t="n">
+      <c r="B158" s="15" t="n">
         <v>45292</v>
       </c>
       <c r="C158" s="0" t="n">
@@ -5414,10 +6572,10 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="n">
+      <c r="A159" s="5" t="n">
         <v>157</v>
       </c>
-      <c r="B159" s="4" t="n">
+      <c r="B159" s="15" t="n">
         <v>45323</v>
       </c>
       <c r="C159" s="0" t="n">
@@ -5440,10 +6598,10 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="n">
+      <c r="A160" s="5" t="n">
         <v>158</v>
       </c>
-      <c r="B160" s="4" t="n">
+      <c r="B160" s="15" t="n">
         <v>45352</v>
       </c>
       <c r="C160" s="0" t="n">
@@ -5466,10 +6624,10 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="n">
+      <c r="A161" s="5" t="n">
         <v>159</v>
       </c>
-      <c r="B161" s="4" t="n">
+      <c r="B161" s="15" t="n">
         <v>45383</v>
       </c>
       <c r="C161" s="0" t="n">
@@ -5492,10 +6650,10 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="n">
+      <c r="A162" s="5" t="n">
         <v>160</v>
       </c>
-      <c r="B162" s="4" t="n">
+      <c r="B162" s="15" t="n">
         <v>45413</v>
       </c>
       <c r="C162" s="0" t="n">
@@ -5518,10 +6676,10 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="n">
+      <c r="A163" s="5" t="n">
         <v>161</v>
       </c>
-      <c r="B163" s="4" t="n">
+      <c r="B163" s="15" t="n">
         <v>45444</v>
       </c>
       <c r="C163" s="0" t="n">
@@ -5561,140 +6719,140 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.7734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>44</v>
+      <c r="A1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>46</v>
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>46</v>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>46</v>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>46</v>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>46</v>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>46</v>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>